<commit_message>
Update specifications in original format
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2_andreas_4.xlsx
+++ b/analysis_specifications/analysis2_andreas_4.xlsx
@@ -437,7 +437,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -501,11 +501,11 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>405</v>
+        <v>765</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Atrial Fibrillation or Flutter</t>
+          <t>Left Heart Failure</t>
         </is>
       </c>
       <c r="C5">
@@ -514,11 +514,11 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>410</v>
+        <v>766</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Acute Urinary tract infections UTI</t>
+          <t>Right Heart Failure</t>
         </is>
       </c>
       <c r="C6">
@@ -527,11 +527,11 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>411</v>
+        <v>795</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sepsis or Septic Shock</t>
+          <t>Antineoplastic drugs against colorectal cancer</t>
         </is>
       </c>
       <c r="C7">
@@ -540,11 +540,11 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>765</v>
+        <v>797</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Left Heart Failure</t>
+          <t>Radiotherapy against colorectal cancer</t>
         </is>
       </c>
       <c r="C8">
@@ -553,11 +553,11 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>766</v>
+        <v>803</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Right Heart Failure</t>
+          <t>Fascial dehiscence and evisceration</t>
         </is>
       </c>
       <c r="C9">
@@ -566,11 +566,11 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>795</v>
+        <v>804</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Antineoplastic drugs against colorectal cancer</t>
+          <t>Anastomotic leak or dehiscence</t>
         </is>
       </c>
       <c r="C10">
@@ -579,11 +579,11 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>797</v>
+        <v>805</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Radiotherapy against colorectal cancer</t>
+          <t>Intestinal obstruction</t>
         </is>
       </c>
       <c r="C11">
@@ -592,11 +592,11 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fascial dehiscence and evisceration</t>
+          <t>Intraabdominal abscess</t>
         </is>
       </c>
       <c r="C12">
@@ -605,11 +605,11 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Anastomotic leak or dehiscence</t>
+          <t>Perioperative aspiration</t>
         </is>
       </c>
       <c r="C13">
@@ -618,11 +618,11 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Intestinal obstruction</t>
+          <t>Postoperative hemorrhage</t>
         </is>
       </c>
       <c r="C14">
@@ -631,11 +631,11 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Intraabdominal abscess</t>
+          <t>Surgical wound infection (narrow)</t>
         </is>
       </c>
       <c r="C15">
@@ -644,11 +644,11 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Perioperative aspiration</t>
+          <t>Distant metastasis following colorectal cancer (wide)</t>
         </is>
       </c>
       <c r="C16">
@@ -657,11 +657,11 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Postoperative hemorrhage</t>
+          <t>Local recurrence after colorectal cancer</t>
         </is>
       </c>
       <c r="C17">
@@ -670,11 +670,11 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>809</v>
+        <v>850</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Surgical wound infection (narrow)</t>
+          <t>Intestinal obstruction</t>
         </is>
       </c>
       <c r="C18">
@@ -683,11 +683,11 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>810</v>
+        <v>851</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Distant metastasis following colorectal cancer (wide)</t>
+          <t>Intraabdominal obstruction</t>
         </is>
       </c>
       <c r="C19">
@@ -696,11 +696,11 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>811</v>
+        <v>852</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Local recurrence after colorectal cancer</t>
+          <t>Surgical wound infection (broad)</t>
         </is>
       </c>
       <c r="C20">
@@ -709,11 +709,11 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Intestinal obstruction</t>
+          <t>Distant metastasis following colorectal cancer (medium)</t>
         </is>
       </c>
       <c r="C21">
@@ -722,11 +722,11 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Intraabdominal obstruction</t>
+          <t>Distant metastasis following colorectal cancer (narrow)</t>
         </is>
       </c>
       <c r="C22">
@@ -735,11 +735,11 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>852</v>
+        <v>861</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Surgical wound infection (broad)</t>
+          <t>Earliest event of Urinary tract infections (UTI)</t>
         </is>
       </c>
       <c r="C23">
@@ -748,11 +748,11 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>854</v>
+        <v>934</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Distant metastasis following colorectal cancer (medium)</t>
+          <t>Persons with heart failure</t>
         </is>
       </c>
       <c r="C24">
@@ -761,92 +761,53 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>855</v>
+        <v>938</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Distant metastasis following colorectal cancer (narrow)</t>
+          <t>Hospitalization with heart failure events</t>
         </is>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>861</v>
+        <v>1081</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Earliest event of Urinary tract infections (UTI)</t>
+          <t>Acute Myocardial Infarction including its complications</t>
         </is>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>934</v>
+        <v>1088</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Persons with heart failure</t>
+          <t>Deep Vein Thrombosis (DVT)</t>
         </is>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>938</v>
+        <v>1090</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Hospitalization with heart failure events</t>
+          <t>Pulmonary Embolism</t>
         </is>
       </c>
       <c r="C28">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>1081</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Acute Myocardial Infarction including its complications</t>
-        </is>
-      </c>
-      <c r="C29">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>1088</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Deep Vein Thrombosis (DVT)</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>1090</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Pulmonary Embolism</t>
-        </is>
-      </c>
-      <c r="C31">
         <v>365</v>
       </c>
     </row>

</xml_diff>